<commit_message>
LB updates - task 22 + task 3a
</commit_message>
<xml_diff>
--- a/srv/handlers/custom_handler/CSV/CountryRiskScores.xlsx
+++ b/srv/handlers/custom_handler/CSV/CountryRiskScores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liviu.stoica\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonard.barascu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AE4433-0A53-4CF5-8247-913D42F2375E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6D7A7D-02E0-084B-AFC5-7D8EA55CD311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{4B6D2A55-92EB-4BCF-A0CC-DC91994B9494}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{4B6D2A55-92EB-4BCF-A0CC-DC91994B9494}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="545">
   <si>
     <t>Region</t>
   </si>
@@ -1668,6 +1668,9 @@
   </si>
   <si>
     <t>ESG02_FundamentalLaborRights</t>
+  </si>
+  <si>
+    <t>LkSG_Activated</t>
   </si>
 </sst>
 </file>
@@ -1724,9 +1727,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1764,7 +1767,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1870,7 +1873,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2012,7 +2015,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2020,31 +2023,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3A610B-15D0-4338-9AC1-D8840D6774D2}">
-  <dimension ref="A1:X250"/>
+  <dimension ref="A1:Y250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>521</v>
       </c>
@@ -2117,8 +2121,11 @@
       <c r="X1" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2191,8 +2198,11 @@
       <c r="X2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2265,8 +2275,11 @@
       <c r="X3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2339,8 +2352,11 @@
       <c r="X4">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2413,8 +2429,11 @@
       <c r="X5">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2487,8 +2506,11 @@
       <c r="X6">
         <v>91</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2561,8 +2583,11 @@
       <c r="X7">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2635,8 +2660,11 @@
       <c r="X8">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2709,8 +2737,11 @@
       <c r="X9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2777,8 +2808,11 @@
       <c r="X10">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2851,8 +2885,11 @@
       <c r="X11">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2925,8 +2962,11 @@
       <c r="X12">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2999,8 +3039,11 @@
       <c r="X13">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -3073,8 +3116,11 @@
       <c r="X14">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -3147,8 +3193,11 @@
       <c r="X15">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -3221,8 +3270,11 @@
       <c r="X16">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -3295,8 +3347,11 @@
       <c r="X17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -3369,8 +3424,11 @@
       <c r="X18">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -3443,8 +3501,11 @@
       <c r="X19">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -3517,8 +3578,11 @@
       <c r="X20">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -3591,8 +3655,11 @@
       <c r="X21">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3665,8 +3732,11 @@
       <c r="X22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3739,8 +3809,11 @@
       <c r="X23">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -3813,8 +3886,11 @@
       <c r="X24">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3887,8 +3963,11 @@
       <c r="X25">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -3961,8 +4040,11 @@
       <c r="X26">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -4035,8 +4117,11 @@
       <c r="X27">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -4109,8 +4194,11 @@
       <c r="X28">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -4183,8 +4271,11 @@
       <c r="X29">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -4257,8 +4348,11 @@
       <c r="X30">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -4331,8 +4425,11 @@
       <c r="X31">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -4405,8 +4502,11 @@
       <c r="X32">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -4479,8 +4579,11 @@
       <c r="X33">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -4553,8 +4656,11 @@
       <c r="X34">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -4627,8 +4733,11 @@
       <c r="X35">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -4701,8 +4810,11 @@
       <c r="X36">
         <v>52</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -4775,8 +4887,11 @@
       <c r="X37">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -4849,8 +4964,11 @@
       <c r="X38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -4923,8 +5041,11 @@
       <c r="X39">
         <v>81</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -4997,8 +5118,11 @@
       <c r="X40">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5071,8 +5195,11 @@
       <c r="X41">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5145,8 +5272,11 @@
       <c r="X42">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -5219,8 +5349,11 @@
       <c r="X43">
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -5293,8 +5426,11 @@
       <c r="X44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -5367,8 +5503,11 @@
       <c r="X45">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>108</v>
       </c>
@@ -5441,8 +5580,11 @@
       <c r="X46">
         <v>51</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>110</v>
       </c>
@@ -5515,8 +5657,11 @@
       <c r="X47">
         <v>28</v>
       </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>113</v>
       </c>
@@ -5589,8 +5734,11 @@
       <c r="X48">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>115</v>
       </c>
@@ -5663,8 +5811,11 @@
       <c r="X49">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>117</v>
       </c>
@@ -5737,8 +5888,11 @@
       <c r="X50">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -5811,8 +5965,11 @@
       <c r="X51">
         <v>39</v>
       </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>121</v>
       </c>
@@ -5885,8 +6042,11 @@
       <c r="X52">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -5959,8 +6119,11 @@
       <c r="X53">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -6033,8 +6196,11 @@
       <c r="X54">
         <v>100</v>
       </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -6107,8 +6273,11 @@
       <c r="X55">
         <v>83</v>
       </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -6181,8 +6350,11 @@
       <c r="X56">
         <v>26</v>
       </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -6255,8 +6427,11 @@
       <c r="X57">
         <v>67</v>
       </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>132</v>
       </c>
@@ -6329,8 +6504,11 @@
       <c r="X58">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>134</v>
       </c>
@@ -6403,8 +6581,11 @@
       <c r="X59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>136</v>
       </c>
@@ -6477,8 +6658,11 @@
       <c r="X60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>138</v>
       </c>
@@ -6551,8 +6735,11 @@
       <c r="X61">
         <v>75</v>
       </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>140</v>
       </c>
@@ -6625,8 +6812,11 @@
       <c r="X62">
         <v>77</v>
       </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>142</v>
       </c>
@@ -6699,8 +6889,11 @@
       <c r="X63">
         <v>27</v>
       </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>144</v>
       </c>
@@ -6773,8 +6966,11 @@
       <c r="X64">
         <v>96</v>
       </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>146</v>
       </c>
@@ -6847,8 +7043,11 @@
       <c r="X65">
         <v>55</v>
       </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -6921,8 +7120,11 @@
       <c r="X66">
         <v>39</v>
       </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>150</v>
       </c>
@@ -6995,8 +7197,11 @@
       <c r="X67">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>152</v>
       </c>
@@ -7069,8 +7274,11 @@
       <c r="X68">
         <v>41</v>
       </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -7143,8 +7351,11 @@
       <c r="X69">
         <v>43</v>
       </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>156</v>
       </c>
@@ -7217,8 +7428,11 @@
       <c r="X70">
         <v>15</v>
       </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>158</v>
       </c>
@@ -7291,8 +7505,11 @@
       <c r="X71">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>160</v>
       </c>
@@ -7365,8 +7582,11 @@
       <c r="X72">
         <v>38</v>
       </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>162</v>
       </c>
@@ -7439,8 +7659,11 @@
       <c r="X73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>164</v>
       </c>
@@ -7513,8 +7736,11 @@
       <c r="X74">
         <v>100</v>
       </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>166</v>
       </c>
@@ -7587,8 +7813,11 @@
       <c r="X75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>168</v>
       </c>
@@ -7661,8 +7890,11 @@
       <c r="X76">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>171</v>
       </c>
@@ -7735,8 +7967,11 @@
       <c r="X77">
         <v>80</v>
       </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>173</v>
       </c>
@@ -7809,8 +8044,11 @@
       <c r="X78">
         <v>56</v>
       </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -7883,8 +8121,11 @@
       <c r="X79">
         <v>100</v>
       </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -7957,8 +8198,11 @@
       <c r="X80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>179</v>
       </c>
@@ -8031,8 +8275,11 @@
       <c r="X81">
         <v>100</v>
       </c>
-    </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>181</v>
       </c>
@@ -8105,8 +8352,11 @@
       <c r="X82">
         <v>50</v>
       </c>
-    </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>183</v>
       </c>
@@ -8179,8 +8429,11 @@
       <c r="X83">
         <v>49</v>
       </c>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>185</v>
       </c>
@@ -8253,8 +8506,11 @@
       <c r="X84">
         <v>29</v>
       </c>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>187</v>
       </c>
@@ -8327,8 +8583,11 @@
       <c r="X85">
         <v>67</v>
       </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>189</v>
       </c>
@@ -8401,8 +8660,11 @@
       <c r="X86">
         <v>44</v>
       </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>191</v>
       </c>
@@ -8475,8 +8737,11 @@
       <c r="X87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>193</v>
       </c>
@@ -8549,8 +8814,11 @@
       <c r="X88">
         <v>49</v>
       </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>195</v>
       </c>
@@ -8623,8 +8891,11 @@
       <c r="X89">
         <v>98</v>
       </c>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>197</v>
       </c>
@@ -8697,8 +8968,11 @@
       <c r="X90">
         <v>85</v>
       </c>
-    </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>199</v>
       </c>
@@ -8771,8 +9045,11 @@
       <c r="X91">
         <v>100</v>
       </c>
-    </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>201</v>
       </c>
@@ -8845,8 +9122,11 @@
       <c r="X92">
         <v>75</v>
       </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>204</v>
       </c>
@@ -8919,8 +9199,11 @@
       <c r="X93">
         <v>35</v>
       </c>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>206</v>
       </c>
@@ -8993,8 +9276,11 @@
       <c r="X94">
         <v>100</v>
       </c>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>208</v>
       </c>
@@ -9067,8 +9353,11 @@
       <c r="X95">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>210</v>
       </c>
@@ -9141,8 +9430,11 @@
       <c r="X96">
         <v>31</v>
       </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>212</v>
       </c>
@@ -9215,8 +9507,11 @@
       <c r="X97">
         <v>47</v>
       </c>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>214</v>
       </c>
@@ -9289,8 +9584,11 @@
       <c r="X98">
         <v>10</v>
       </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>216</v>
       </c>
@@ -9363,8 +9661,11 @@
       <c r="X99">
         <v>100</v>
       </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>218</v>
       </c>
@@ -9437,8 +9738,11 @@
       <c r="X100">
         <v>100</v>
       </c>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>220</v>
       </c>
@@ -9511,8 +9815,11 @@
       <c r="X101">
         <v>25</v>
       </c>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>222</v>
       </c>
@@ -9585,8 +9892,11 @@
       <c r="X102">
         <v>67</v>
       </c>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>224</v>
       </c>
@@ -9659,8 +9969,11 @@
       <c r="X103">
         <v>68</v>
       </c>
-    </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>226</v>
       </c>
@@ -9733,8 +10046,11 @@
       <c r="X104">
         <v>95</v>
       </c>
-    </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>228</v>
       </c>
@@ -9807,8 +10123,11 @@
       <c r="X105">
         <v>25</v>
       </c>
-    </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>230</v>
       </c>
@@ -9881,8 +10200,11 @@
       <c r="X106">
         <v>29</v>
       </c>
-    </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>232</v>
       </c>
@@ -9955,8 +10277,11 @@
       <c r="X107">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>234</v>
       </c>
@@ -10029,8 +10354,11 @@
       <c r="X108">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>236</v>
       </c>
@@ -10103,8 +10431,11 @@
       <c r="X109">
         <v>79</v>
       </c>
-    </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>238</v>
       </c>
@@ -10177,8 +10508,11 @@
       <c r="X110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>240</v>
       </c>
@@ -10251,8 +10585,11 @@
       <c r="X111">
         <v>12</v>
       </c>
-    </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>242</v>
       </c>
@@ -10325,8 +10662,11 @@
       <c r="X112">
         <v>58</v>
       </c>
-    </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>244</v>
       </c>
@@ -10399,8 +10739,11 @@
       <c r="X113">
         <v>58</v>
       </c>
-    </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>246</v>
       </c>
@@ -10473,8 +10816,11 @@
       <c r="X114">
         <v>87</v>
       </c>
-    </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>248</v>
       </c>
@@ -10547,8 +10893,11 @@
       <c r="X115">
         <v>100</v>
       </c>
-    </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>250</v>
       </c>
@@ -10621,8 +10970,11 @@
       <c r="X116">
         <v>35</v>
       </c>
-    </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>252</v>
       </c>
@@ -10695,8 +11047,11 @@
       <c r="X117">
         <v>33</v>
       </c>
-    </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>255</v>
       </c>
@@ -10769,8 +11124,11 @@
       <c r="X118">
         <v>15</v>
       </c>
-    </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>257</v>
       </c>
@@ -10843,8 +11201,11 @@
       <c r="X119">
         <v>90</v>
       </c>
-    </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>259</v>
       </c>
@@ -10917,8 +11278,11 @@
       <c r="X120">
         <v>30</v>
       </c>
-    </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>261</v>
       </c>
@@ -10991,8 +11355,11 @@
       <c r="X121">
         <v>65</v>
       </c>
-    </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>263</v>
       </c>
@@ -11065,8 +11432,11 @@
       <c r="X122">
         <v>54</v>
       </c>
-    </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>265</v>
       </c>
@@ -11139,8 +11509,11 @@
       <c r="X123">
         <v>25</v>
       </c>
-    </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>267</v>
       </c>
@@ -11213,8 +11586,11 @@
       <c r="X124">
         <v>74</v>
       </c>
-    </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>269</v>
       </c>
@@ -11287,8 +11663,11 @@
       <c r="X125">
         <v>60</v>
       </c>
-    </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>271</v>
       </c>
@@ -11361,8 +11740,11 @@
       <c r="X126">
         <v>9</v>
       </c>
-    </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>273</v>
       </c>
@@ -11435,8 +11817,11 @@
       <c r="X127">
         <v>42</v>
       </c>
-    </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>275</v>
       </c>
@@ -11509,8 +11894,11 @@
       <c r="X128">
         <v>36</v>
       </c>
-    </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>277</v>
       </c>
@@ -11583,8 +11971,11 @@
       <c r="X129">
         <v>4</v>
       </c>
-    </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>279</v>
       </c>
@@ -11657,8 +12048,11 @@
       <c r="X130">
         <v>100</v>
       </c>
-    </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>281</v>
       </c>
@@ -11731,8 +12125,11 @@
       <c r="X131">
         <v>69</v>
       </c>
-    </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>283</v>
       </c>
@@ -11805,8 +12202,11 @@
       <c r="X132">
         <v>86</v>
       </c>
-    </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>285</v>
       </c>
@@ -11879,8 +12279,11 @@
       <c r="X133">
         <v>90</v>
       </c>
-    </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>287</v>
       </c>
@@ -11953,8 +12356,11 @@
       <c r="X134">
         <v>26</v>
       </c>
-    </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>289</v>
       </c>
@@ -12027,8 +12433,11 @@
       <c r="X135">
         <v>42</v>
       </c>
-    </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>291</v>
       </c>
@@ -12101,8 +12510,11 @@
       <c r="X136">
         <v>52</v>
       </c>
-    </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>293</v>
       </c>
@@ -12175,8 +12587,11 @@
       <c r="X137">
         <v>70</v>
       </c>
-    </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>295</v>
       </c>
@@ -12249,8 +12664,11 @@
       <c r="X138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>297</v>
       </c>
@@ -12323,8 +12741,11 @@
       <c r="X139">
         <v>81</v>
       </c>
-    </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>299</v>
       </c>
@@ -12397,8 +12818,11 @@
       <c r="X140">
         <v>86</v>
       </c>
-    </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>301</v>
       </c>
@@ -12471,8 +12895,11 @@
       <c r="X141">
         <v>100</v>
       </c>
-    </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>303</v>
       </c>
@@ -12545,8 +12972,11 @@
       <c r="X142">
         <v>27</v>
       </c>
-    </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>305</v>
       </c>
@@ -12619,8 +13049,11 @@
       <c r="X143">
         <v>75</v>
       </c>
-    </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>307</v>
       </c>
@@ -12693,8 +13126,11 @@
       <c r="X144">
         <v>100</v>
       </c>
-    </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>309</v>
       </c>
@@ -12767,8 +13203,11 @@
       <c r="X145">
         <v>22</v>
       </c>
-    </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>311</v>
       </c>
@@ -12841,8 +13280,11 @@
       <c r="X146">
         <v>94</v>
       </c>
-    </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>313</v>
       </c>
@@ -12915,8 +13357,11 @@
       <c r="X147">
         <v>22</v>
       </c>
-    </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>315</v>
       </c>
@@ -12989,8 +13434,11 @@
       <c r="X148">
         <v>94</v>
       </c>
-    </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>317</v>
       </c>
@@ -13063,8 +13511,11 @@
       <c r="X149">
         <v>63</v>
       </c>
-    </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>319</v>
       </c>
@@ -13137,8 +13588,11 @@
       <c r="X150">
         <v>44</v>
       </c>
-    </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>321</v>
       </c>
@@ -13211,8 +13665,11 @@
       <c r="X151">
         <v>100</v>
       </c>
-    </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>323</v>
       </c>
@@ -13285,8 +13742,11 @@
       <c r="X152">
         <v>34</v>
       </c>
-    </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>325</v>
       </c>
@@ -13359,8 +13819,11 @@
       <c r="X153">
         <v>11</v>
       </c>
-    </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>327</v>
       </c>
@@ -13433,8 +13896,11 @@
       <c r="X154">
         <v>3</v>
       </c>
-    </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>329</v>
       </c>
@@ -13507,8 +13973,11 @@
       <c r="X155">
         <v>64</v>
       </c>
-    </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>331</v>
       </c>
@@ -13581,8 +14050,11 @@
       <c r="X156">
         <v>78</v>
       </c>
-    </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>333</v>
       </c>
@@ -13655,8 +14127,11 @@
       <c r="X157">
         <v>38</v>
       </c>
-    </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>335</v>
       </c>
@@ -13729,8 +14204,11 @@
       <c r="X158">
         <v>71</v>
       </c>
-    </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>337</v>
       </c>
@@ -13803,8 +14281,11 @@
       <c r="X159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>339</v>
       </c>
@@ -13877,8 +14358,11 @@
       <c r="X160">
         <v>96</v>
       </c>
-    </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>341</v>
       </c>
@@ -13951,8 +14435,11 @@
       <c r="X161">
         <v>33</v>
       </c>
-    </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>343</v>
       </c>
@@ -14025,8 +14512,11 @@
       <c r="X162">
         <v>10</v>
       </c>
-    </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>345</v>
       </c>
@@ -14099,8 +14589,11 @@
       <c r="X163">
         <v>8</v>
       </c>
-    </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>347</v>
       </c>
@@ -14173,8 +14666,11 @@
       <c r="X164">
         <v>100</v>
       </c>
-    </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>349</v>
       </c>
@@ -14247,8 +14743,11 @@
       <c r="X165">
         <v>100</v>
       </c>
-    </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>351</v>
       </c>
@@ -14321,8 +14820,11 @@
       <c r="X166">
         <v>51</v>
       </c>
-    </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>353</v>
       </c>
@@ -14395,8 +14897,11 @@
       <c r="X167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>355</v>
       </c>
@@ -14469,8 +14974,11 @@
       <c r="X168">
         <v>76</v>
       </c>
-    </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>357</v>
       </c>
@@ -14543,8 +15051,11 @@
       <c r="X169">
         <v>63</v>
       </c>
-    </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>359</v>
       </c>
@@ -14617,8 +15128,11 @@
       <c r="X170">
         <v>7</v>
       </c>
-    </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>361</v>
       </c>
@@ -14691,8 +15205,11 @@
       <c r="X171">
         <v>89</v>
       </c>
-    </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>363</v>
       </c>
@@ -14765,8 +15282,11 @@
       <c r="X172">
         <v>7</v>
       </c>
-    </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>365</v>
       </c>
@@ -14839,8 +15359,11 @@
       <c r="X173">
         <v>55</v>
       </c>
-    </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>367</v>
       </c>
@@ -14913,8 +15436,11 @@
       <c r="X174">
         <v>24</v>
       </c>
-    </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>369</v>
       </c>
@@ -14987,8 +15513,11 @@
       <c r="X175">
         <v>48</v>
       </c>
-    </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>371</v>
       </c>
@@ -15061,8 +15590,11 @@
       <c r="X176">
         <v>28</v>
       </c>
-    </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>373</v>
       </c>
@@ -15135,8 +15667,11 @@
       <c r="X177">
         <v>20</v>
       </c>
-    </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>375</v>
       </c>
@@ -15209,8 +15744,11 @@
       <c r="X178">
         <v>100</v>
       </c>
-    </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>377</v>
       </c>
@@ -15283,8 +15821,11 @@
       <c r="X179">
         <v>62</v>
       </c>
-    </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>379</v>
       </c>
@@ -15357,8 +15898,11 @@
       <c r="X180">
         <v>76</v>
       </c>
-    </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>381</v>
       </c>
@@ -15431,8 +15975,11 @@
       <c r="X181">
         <v>64</v>
       </c>
-    </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>383</v>
       </c>
@@ -15505,8 +16052,11 @@
       <c r="X182">
         <v>84</v>
       </c>
-    </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>385</v>
       </c>
@@ -15579,8 +16129,11 @@
       <c r="X183">
         <v>100</v>
       </c>
-    </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>387</v>
       </c>
@@ -15653,8 +16206,11 @@
       <c r="X184">
         <v>61</v>
       </c>
-    </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>389</v>
       </c>
@@ -15727,8 +16283,11 @@
       <c r="X185">
         <v>16</v>
       </c>
-    </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>391</v>
       </c>
@@ -15801,8 +16360,11 @@
       <c r="X186">
         <v>48</v>
       </c>
-    </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>393</v>
       </c>
@@ -15875,8 +16437,11 @@
       <c r="X187">
         <v>100</v>
       </c>
-    </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>395</v>
       </c>
@@ -15946,8 +16511,11 @@
       <c r="X188">
         <v>100</v>
       </c>
-    </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>397</v>
       </c>
@@ -16020,8 +16588,11 @@
       <c r="X189">
         <v>83</v>
       </c>
-    </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>399</v>
       </c>
@@ -16094,8 +16665,11 @@
       <c r="X190">
         <v>78</v>
       </c>
-    </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>401</v>
       </c>
@@ -16168,8 +16742,11 @@
       <c r="X191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>403</v>
       </c>
@@ -16242,8 +16819,11 @@
       <c r="X192">
         <v>100</v>
       </c>
-    </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>405</v>
       </c>
@@ -16316,8 +16896,11 @@
       <c r="X193">
         <v>85</v>
       </c>
-    </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>407</v>
       </c>
@@ -16390,8 +16973,11 @@
       <c r="X194">
         <v>88</v>
       </c>
-    </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>409</v>
       </c>
@@ -16464,8 +17050,11 @@
       <c r="X195">
         <v>94</v>
       </c>
-    </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>411</v>
       </c>
@@ -16538,8 +17127,11 @@
       <c r="X196">
         <v>66</v>
       </c>
-    </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>413</v>
       </c>
@@ -16612,8 +17204,11 @@
       <c r="X197">
         <v>32</v>
       </c>
-    </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>415</v>
       </c>
@@ -16686,8 +17281,11 @@
       <c r="X198">
         <v>41</v>
       </c>
-    </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>417</v>
       </c>
@@ -16760,8 +17358,11 @@
       <c r="X199">
         <v>40</v>
       </c>
-    </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>419</v>
       </c>
@@ -16834,8 +17435,11 @@
       <c r="X200">
         <v>73</v>
       </c>
-    </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>421</v>
       </c>
@@ -16908,8 +17512,11 @@
       <c r="X201">
         <v>43</v>
       </c>
-    </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>423</v>
       </c>
@@ -16982,8 +17589,11 @@
       <c r="X202">
         <v>97</v>
       </c>
-    </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>425</v>
       </c>
@@ -17056,8 +17666,11 @@
       <c r="X203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>427</v>
       </c>
@@ -17130,8 +17743,11 @@
       <c r="X204">
         <v>60</v>
       </c>
-    </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>429</v>
       </c>
@@ -17204,8 +17820,11 @@
       <c r="X205">
         <v>71</v>
       </c>
-    </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>431</v>
       </c>
@@ -17278,8 +17897,11 @@
       <c r="X206">
         <v>57</v>
       </c>
-    </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>433</v>
       </c>
@@ -17352,8 +17974,11 @@
       <c r="X207">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>435</v>
       </c>
@@ -17426,8 +18051,11 @@
       <c r="X208">
         <v>20</v>
       </c>
-    </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>437</v>
       </c>
@@ -17500,8 +18128,11 @@
       <c r="X209">
         <v>100</v>
       </c>
-    </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>439</v>
       </c>
@@ -17574,8 +18205,11 @@
       <c r="X210">
         <v>3</v>
       </c>
-    </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>441</v>
       </c>
@@ -17648,8 +18282,11 @@
       <c r="X211">
         <v>53</v>
       </c>
-    </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>443</v>
       </c>
@@ -17722,8 +18359,11 @@
       <c r="X212">
         <v>19</v>
       </c>
-    </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>445</v>
       </c>
@@ -17796,8 +18436,11 @@
       <c r="X213">
         <v>5</v>
       </c>
-    </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>447</v>
       </c>
@@ -17870,8 +18513,11 @@
       <c r="X214">
         <v>58</v>
       </c>
-    </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>449</v>
       </c>
@@ -17944,8 +18590,11 @@
       <c r="X215">
         <v>100</v>
       </c>
-    </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>451</v>
       </c>
@@ -18018,8 +18667,11 @@
       <c r="X216">
         <v>80</v>
       </c>
-    </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>453</v>
       </c>
@@ -18092,8 +18744,11 @@
       <c r="X217">
         <v>92</v>
       </c>
-    </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>455</v>
       </c>
@@ -18166,8 +18821,11 @@
       <c r="X218">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>457</v>
       </c>
@@ -18240,8 +18898,11 @@
       <c r="X219">
         <v>100</v>
       </c>
-    </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>459</v>
       </c>
@@ -18314,8 +18975,11 @@
       <c r="X220">
         <v>21</v>
       </c>
-    </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>461</v>
       </c>
@@ -18385,8 +19049,11 @@
       <c r="X221">
         <v>37</v>
       </c>
-    </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>463</v>
       </c>
@@ -18459,8 +19126,11 @@
       <c r="X222">
         <v>32</v>
       </c>
-    </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>465</v>
       </c>
@@ -18533,8 +19203,11 @@
       <c r="X223">
         <v>54</v>
       </c>
-    </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>467</v>
       </c>
@@ -18607,8 +19280,11 @@
       <c r="X224">
         <v>21</v>
       </c>
-    </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>469</v>
       </c>
@@ -18681,8 +19357,11 @@
       <c r="X225">
         <v>100</v>
       </c>
-    </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>471</v>
       </c>
@@ -18755,8 +19434,11 @@
       <c r="X226">
         <v>89</v>
       </c>
-    </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>473</v>
       </c>
@@ -18829,8 +19511,11 @@
       <c r="X227">
         <v>57</v>
       </c>
-    </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>475</v>
       </c>
@@ -18903,8 +19588,11 @@
       <c r="X228">
         <v>24</v>
       </c>
-    </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>477</v>
       </c>
@@ -18977,8 +19665,11 @@
       <c r="X229">
         <v>14</v>
       </c>
-    </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>479</v>
       </c>
@@ -19051,8 +19742,11 @@
       <c r="X230">
         <v>42</v>
       </c>
-    </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>481</v>
       </c>
@@ -19125,8 +19819,11 @@
       <c r="X231">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>483</v>
       </c>
@@ -19199,8 +19896,11 @@
       <c r="X232">
         <v>93</v>
       </c>
-    </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>485</v>
       </c>
@@ -19273,8 +19973,11 @@
       <c r="X233">
         <v>17</v>
       </c>
-    </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>487</v>
       </c>
@@ -19347,8 +20050,11 @@
       <c r="X234">
         <v>6</v>
       </c>
-    </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>489</v>
       </c>
@@ -19421,8 +20127,11 @@
       <c r="X235">
         <v>70</v>
       </c>
-    </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>491</v>
       </c>
@@ -19495,8 +20204,11 @@
       <c r="X236">
         <v>62</v>
       </c>
-    </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>493</v>
       </c>
@@ -19569,8 +20281,11 @@
       <c r="X237">
         <v>45</v>
       </c>
-    </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>495</v>
       </c>
@@ -19643,8 +20358,11 @@
       <c r="X238">
         <v>100</v>
       </c>
-    </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>497</v>
       </c>
@@ -19717,8 +20435,11 @@
       <c r="X239">
         <v>88</v>
       </c>
-    </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>499</v>
       </c>
@@ -19791,8 +20512,11 @@
       <c r="X240">
         <v>40</v>
       </c>
-    </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>501</v>
       </c>
@@ -19865,8 +20589,11 @@
       <c r="X241">
         <v>83</v>
       </c>
-    </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>503</v>
       </c>
@@ -19939,8 +20666,11 @@
       <c r="X242">
         <v>12</v>
       </c>
-    </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>505</v>
       </c>
@@ -20013,8 +20743,11 @@
       <c r="X243">
         <v>46</v>
       </c>
-    </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>507</v>
       </c>
@@ -20087,8 +20820,11 @@
       <c r="X244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>509</v>
       </c>
@@ -20161,8 +20897,11 @@
       <c r="X245">
         <v>65</v>
       </c>
-    </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>511</v>
       </c>
@@ -20235,8 +20974,11 @@
       <c r="X246">
         <v>100</v>
       </c>
-    </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>513</v>
       </c>
@@ -20309,8 +21051,11 @@
       <c r="X247">
         <v>100</v>
       </c>
-    </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>515</v>
       </c>
@@ -20383,8 +21128,11 @@
       <c r="X248">
         <v>2</v>
       </c>
-    </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>517</v>
       </c>
@@ -20457,8 +21205,11 @@
       <c r="X249">
         <v>50</v>
       </c>
-    </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>519</v>
       </c>
@@ -20530,6 +21281,9 @@
       </c>
       <c r="X250">
         <v>17</v>
+      </c>
+      <c r="Y250">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>